<commit_message>
a24:added report draft; merged optimization
</commit_message>
<xml_diff>
--- a/A2.4/data/optimization1/posl-optimization1.xlsx
+++ b/A2.4/data/optimization1/posl-optimization1.xlsx
@@ -31,9 +31,6 @@
     <t>Scalability</t>
   </si>
   <si>
-    <t>Data exch (bytes)</t>
-  </si>
-  <si>
     <t>-03 optimization</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Scalability</t>
   </si>
   <si>
-    <t>Data exch (bytes)</t>
-  </si>
-  <si>
     <t>-03 optimization</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
   </si>
   <si>
     <t>Scalability</t>
-  </si>
-  <si>
-    <t>Data exch (bytes)</t>
   </si>
   <si>
     <t>-03 optimization</t>
@@ -98,9 +89,6 @@
   </si>
   <si>
     <t>Scalability</t>
-  </si>
-  <si>
-    <t>Data exch (bytes)</t>
   </si>
 </sst>
 </file>
@@ -322,9 +310,7 @@
       <c t="s" s="5" r="A2">
         <v>3</v>
       </c>
-      <c s="5" r="B2">
-        <v>1.0</v>
-      </c>
+      <c s="5" r="B2"/>
       <c s="5" r="C2">
         <v>2.0</v>
       </c>
@@ -375,9 +361,7 @@
       <c s="7" r="A3">
         <v>1.0</v>
       </c>
-      <c s="8" r="B3">
-        <v>0.072927</v>
-      </c>
+      <c s="8" r="B3"/>
       <c s="8" r="C3">
         <v>0.207009</v>
       </c>
@@ -428,9 +412,7 @@
       <c s="7" r="A4">
         <v>2.0</v>
       </c>
-      <c s="8" r="B4">
-        <v>0.057504</v>
-      </c>
+      <c s="8" r="B4"/>
       <c s="8" r="C4">
         <v>0.208498</v>
       </c>
@@ -481,9 +463,7 @@
       <c s="7" r="A5">
         <v>3.0</v>
       </c>
-      <c s="8" r="B5">
-        <v>0.057323</v>
-      </c>
+      <c s="8" r="B5"/>
       <c s="8" r="C5">
         <v>0.206077</v>
       </c>
@@ -534,12 +514,9 @@
       <c t="s" s="9" r="A6">
         <v>4</v>
       </c>
-      <c t="str" s="10" r="B6">
-        <f ref="B6:I6" t="shared" si="1">AVERAGE(B3:B5)</f>
-        <v>0.06258466667</v>
-      </c>
+      <c s="10" r="B6"/>
       <c t="str" s="10" r="C6">
-        <f t="shared" si="1"/>
+        <f ref="C6:I6" t="shared" si="1">AVERAGE(C3:C5)</f>
         <v>0.2071946667</v>
       </c>
       <c t="str" s="10" r="D6">
@@ -595,37 +572,34 @@
       <c t="s" s="7" r="A7">
         <v>5</v>
       </c>
-      <c t="str" s="11" r="B7">
-        <f>DIVIDE(B6, B6)</f>
+      <c s="11" r="B7"/>
+      <c t="str" s="11" r="C7">
+        <f>DIVIDE(C6, C6)</f>
         <v>1</v>
       </c>
-      <c t="str" s="11" r="C7">
-        <f>DIVIDE(B6, C6)</f>
-        <v>0.3020573245</v>
-      </c>
       <c t="str" s="11" r="D7">
-        <f>DIVIDE(B6, D6)</f>
-        <v>0.2837744906</v>
+        <f>DIVIDE(C6, D6)</f>
+        <v>0.939472304</v>
       </c>
       <c t="str" s="11" r="E7">
-        <f>DIVIDE(B6, E6)</f>
-        <v>0.2685184391</v>
+        <f>DIVIDE(C6, E6)</f>
+        <v>0.8889651641</v>
       </c>
       <c t="str" s="11" r="F7">
-        <f>DIVIDE(B6, F6)</f>
-        <v>0.2659333531</v>
+        <f>DIVIDE(C6, F6)</f>
+        <v>0.8804069012</v>
       </c>
       <c t="str" s="11" r="G7">
-        <f>DIVIDE(B6, G6)</f>
-        <v>0.2506079867</v>
+        <f>DIVIDE(C6, G6)</f>
+        <v>0.8296702857</v>
       </c>
       <c t="str" s="11" r="H7">
-        <f>DIVIDE(B6, H6)</f>
-        <v>0.236488929</v>
+        <f>DIVIDE(C6, H6)</f>
+        <v>0.7829273116</v>
       </c>
       <c t="str" s="11" r="I7">
-        <f>DIVIDE(B6, I6)</f>
-        <v>0.2272715168</v>
+        <f>DIVIDE(C6, I6)</f>
+        <v>0.7524118714</v>
       </c>
       <c s="6" r="J7"/>
       <c s="6" r="K7"/>
@@ -653,33 +627,15 @@
       <c s="6" r="AG7"/>
     </row>
     <row r="8">
-      <c t="s" s="7" r="A8">
-        <v>6</v>
-      </c>
-      <c s="8" r="B8">
-        <v>0.0</v>
-      </c>
-      <c s="12" r="C8">
-        <v>7560.0</v>
-      </c>
-      <c s="12" r="D8">
-        <v>9060.0</v>
-      </c>
-      <c s="12" r="E8">
-        <v>13700.0</v>
-      </c>
-      <c s="12" r="F8">
-        <v>17400.0</v>
-      </c>
-      <c s="12" r="G8">
-        <v>19500.0</v>
-      </c>
-      <c s="12" r="H8">
-        <v>21100.0</v>
-      </c>
-      <c s="12" r="I8">
-        <v>24800.0</v>
-      </c>
+      <c s="7" r="A8"/>
+      <c s="8" r="B8"/>
+      <c s="12" r="C8"/>
+      <c s="12" r="D8"/>
+      <c s="12" r="E8"/>
+      <c s="12" r="F8"/>
+      <c s="12" r="G8"/>
+      <c s="12" r="H8"/>
+      <c s="12" r="I8"/>
       <c s="4" r="J8"/>
       <c s="4" r="K8"/>
       <c s="4" r="L8"/>
@@ -742,16 +698,16 @@
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
+        <v>6</v>
+      </c>
+      <c t="s" s="2" r="B10">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="B10">
+      <c t="s" s="3" r="C10">
         <v>8</v>
       </c>
-      <c t="s" s="3" r="C10">
+      <c t="s" s="14" r="D10">
         <v>9</v>
-      </c>
-      <c t="s" s="14" r="D10">
-        <v>10</v>
       </c>
       <c s="4" r="E10"/>
       <c s="4" r="F10"/>
@@ -785,11 +741,9 @@
     </row>
     <row r="11">
       <c t="s" s="5" r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
-      <c s="5" r="B11">
-        <v>1.0</v>
-      </c>
+      <c s="5" r="B11"/>
       <c s="5" r="C11">
         <v>2.0</v>
       </c>
@@ -840,9 +794,7 @@
       <c s="7" r="A12">
         <v>1.0</v>
       </c>
-      <c s="8" r="B12">
-        <v>0.072927</v>
-      </c>
+      <c s="8" r="B12"/>
       <c s="15" r="C12">
         <v>0.202496</v>
       </c>
@@ -893,9 +845,7 @@
       <c s="7" r="A13">
         <v>2.0</v>
       </c>
-      <c s="8" r="B13">
-        <v>0.057504</v>
-      </c>
+      <c s="8" r="B13"/>
       <c s="15" r="C13">
         <v>0.200487</v>
       </c>
@@ -946,9 +896,7 @@
       <c s="7" r="A14">
         <v>3.0</v>
       </c>
-      <c s="8" r="B14">
-        <v>0.057323</v>
-      </c>
+      <c s="8" r="B14"/>
       <c s="15" r="C14">
         <v>0.200732</v>
       </c>
@@ -997,14 +945,11 @@
     </row>
     <row r="15">
       <c t="s" s="9" r="A15">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c t="str" s="10" r="B15">
-        <f ref="B15:I15" t="shared" si="2">AVERAGE(B12:B14)</f>
-        <v>0.06258466667</v>
-      </c>
+      <c s="10" r="B15"/>
       <c t="str" s="10" r="C15">
-        <f t="shared" si="2"/>
+        <f ref="C15:I15" t="shared" si="2">AVERAGE(C12:C14)</f>
         <v>0.2012383333</v>
       </c>
       <c t="str" s="10" r="D15">
@@ -1058,39 +1003,36 @@
     </row>
     <row r="16">
       <c t="s" s="7" r="A16">
-        <v>13</v>
+        <v>12</v>
       </c>
-      <c t="str" s="11" r="B16">
-        <f>DIVIDE(B15, B15)</f>
+      <c s="11" r="B16"/>
+      <c t="str" s="11" r="C16">
+        <f>DIVIDE(C15, C15)</f>
         <v>1</v>
       </c>
-      <c t="str" s="11" r="C16">
-        <f>DIVIDE(B15, C15)</f>
-        <v>0.310997739</v>
-      </c>
       <c t="str" s="11" r="D16">
-        <f>DIVIDE(B15, D15)</f>
-        <v>0.2984215387</v>
+        <f>DIVIDE(C15, D15)</f>
+        <v>0.9595617628</v>
       </c>
       <c t="str" s="11" r="E16">
-        <f>DIVIDE(B15, E15)</f>
-        <v>0.2940322512</v>
+        <f>DIVIDE(C15, E15)</f>
+        <v>0.9454481958</v>
       </c>
       <c t="str" s="11" r="F16">
-        <f>DIVIDE(B15, F15)</f>
-        <v>0.2782051814</v>
+        <f>DIVIDE(C15, F15)</f>
+        <v>0.894556926</v>
       </c>
       <c t="str" s="11" r="G16">
-        <f>DIVIDE(B15, G15)</f>
-        <v>0.263675737</v>
+        <f>DIVIDE(C15, G15)</f>
+        <v>0.8478381157</v>
       </c>
       <c t="str" s="11" r="H16">
-        <f>DIVIDE(B15, H15)</f>
-        <v>0.2347858274</v>
+        <f>DIVIDE(C15, H15)</f>
+        <v>0.7549438402</v>
       </c>
       <c t="str" s="11" r="I16">
-        <f>DIVIDE(B15, I15)</f>
-        <v>0.2296758062</v>
+        <f>DIVIDE(C15, I15)</f>
+        <v>0.7385127845</v>
       </c>
       <c s="6" r="J16"/>
       <c s="6" r="K16"/>
@@ -1118,33 +1060,15 @@
       <c s="6" r="AG16"/>
     </row>
     <row r="17">
-      <c t="s" s="7" r="A17">
-        <v>14</v>
-      </c>
-      <c s="8" r="B17">
-        <v>0.0</v>
-      </c>
-      <c s="12" r="C17">
-        <v>7560.0</v>
-      </c>
-      <c s="12" r="D17">
-        <v>9060.0</v>
-      </c>
-      <c s="12" r="E17">
-        <v>13700.0</v>
-      </c>
-      <c s="12" r="F17">
-        <v>17400.0</v>
-      </c>
-      <c s="12" r="G17">
-        <v>19500.0</v>
-      </c>
-      <c s="12" r="H17">
-        <v>21100.0</v>
-      </c>
-      <c s="12" r="I17">
-        <v>24800.0</v>
-      </c>
+      <c s="7" r="A17"/>
+      <c s="8" r="B17"/>
+      <c s="12" r="C17"/>
+      <c s="12" r="D17"/>
+      <c s="12" r="E17"/>
+      <c s="12" r="F17"/>
+      <c s="12" r="G17"/>
+      <c s="12" r="H17"/>
+      <c s="12" r="I17"/>
       <c s="4" r="J17"/>
       <c s="4" r="K17"/>
       <c s="4" r="L17"/>
@@ -1207,13 +1131,13 @@
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c t="s" s="2" r="B19">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c t="s" s="3" r="C19">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c s="4" r="D19"/>
       <c s="4" r="E19"/>
@@ -1248,11 +1172,9 @@
     </row>
     <row r="20">
       <c t="s" s="5" r="A20">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c s="5" r="B20">
-        <v>1.0</v>
-      </c>
+      <c s="5" r="B20"/>
       <c s="5" r="C20">
         <v>2.0</v>
       </c>
@@ -1303,9 +1225,7 @@
       <c s="7" r="A21">
         <v>1.0</v>
       </c>
-      <c s="8" r="B21">
-        <v>0.532166</v>
-      </c>
+      <c s="8" r="B21"/>
       <c s="8" r="C21">
         <v>1.579172</v>
       </c>
@@ -1356,9 +1276,7 @@
       <c s="7" r="A22">
         <v>2.0</v>
       </c>
-      <c s="8" r="B22">
-        <v>0.374772</v>
-      </c>
+      <c s="8" r="B22"/>
       <c s="8" r="C22">
         <v>1.577735</v>
       </c>
@@ -1409,9 +1327,7 @@
       <c s="7" r="A23">
         <v>3.0</v>
       </c>
-      <c s="8" r="B23">
-        <v>0.37328</v>
-      </c>
+      <c s="8" r="B23"/>
       <c s="8" r="C23">
         <v>1.576239</v>
       </c>
@@ -1460,14 +1376,11 @@
     </row>
     <row r="24">
       <c t="s" s="9" r="A24">
-        <v>19</v>
+        <v>17</v>
       </c>
-      <c t="str" s="10" r="B24">
-        <f ref="B24:I24" t="shared" si="3">AVERAGE(B21:B23)</f>
-        <v>0.4267393333</v>
-      </c>
+      <c s="10" r="B24"/>
       <c t="str" s="10" r="C24">
-        <f t="shared" si="3"/>
+        <f ref="C24:I24" t="shared" si="3">AVERAGE(C21:C23)</f>
         <v>1.577715333</v>
       </c>
       <c t="str" s="10" r="D24">
@@ -1521,39 +1434,36 @@
     </row>
     <row r="25">
       <c t="s" s="7" r="A25">
-        <v>20</v>
+        <v>18</v>
       </c>
-      <c t="str" s="11" r="B25">
-        <f>DIVIDE(B24, B24)</f>
+      <c s="11" r="B25"/>
+      <c t="str" s="11" r="C25">
+        <f ref="C25:I25" t="shared" si="4">DIVIDE($C$24, C24)</f>
         <v>1</v>
       </c>
-      <c t="str" s="11" r="C25">
-        <f>DIVIDE(B24, C24)</f>
-        <v>0.2704792964</v>
-      </c>
       <c t="str" s="11" r="D25">
-        <f>DIVIDE(B24, D24)</f>
-        <v>0.2476451602</v>
+        <f t="shared" si="4"/>
+        <v>0.9155789867</v>
       </c>
       <c t="str" s="11" r="E25">
-        <f>DIVIDE(B24, E24)</f>
-        <v>0.2516039971</v>
+        <f t="shared" si="4"/>
+        <v>0.9302153639</v>
       </c>
       <c t="str" s="11" r="F25">
-        <f>DIVIDE(B24, F24)</f>
-        <v>0.2434541478</v>
+        <f t="shared" si="4"/>
+        <v>0.9000842246</v>
       </c>
       <c t="str" s="11" r="G25">
-        <f>DIVIDE(B24, G24)</f>
-        <v>0.2314172417</v>
+        <f t="shared" si="4"/>
+        <v>0.8555820897</v>
       </c>
       <c t="str" s="11" r="H25">
-        <f>DIVIDE(B24, H24)</f>
-        <v>0.2244962627</v>
+        <f t="shared" si="4"/>
+        <v>0.829994257</v>
       </c>
       <c t="str" s="11" r="I25">
-        <f>DIVIDE(B24, I24)</f>
-        <v>0.2211809292</v>
+        <f t="shared" si="4"/>
+        <v>0.817737003</v>
       </c>
       <c s="6" r="J25"/>
       <c s="6" r="K25"/>
@@ -1581,33 +1491,15 @@
       <c s="6" r="AG25"/>
     </row>
     <row r="26">
-      <c t="s" s="7" r="A26">
-        <v>21</v>
-      </c>
-      <c s="8" r="B26">
-        <v>0.0</v>
-      </c>
-      <c s="12" r="C26">
-        <v>18600.0</v>
-      </c>
-      <c s="12" r="D26">
-        <v>44300.0</v>
-      </c>
-      <c s="12" r="E26">
-        <v>55300.0</v>
-      </c>
-      <c s="12" r="F26">
-        <v>65500.0</v>
-      </c>
-      <c s="12" r="G26">
-        <v>76300.0</v>
-      </c>
-      <c s="12" r="H26">
-        <v>81700.0</v>
-      </c>
-      <c s="12" r="I26">
-        <v>91300.0</v>
-      </c>
+      <c s="7" r="A26"/>
+      <c s="8" r="B26"/>
+      <c s="12" r="C26"/>
+      <c s="12" r="D26"/>
+      <c s="12" r="E26"/>
+      <c s="12" r="F26"/>
+      <c s="12" r="G26"/>
+      <c s="12" r="H26"/>
+      <c s="12" r="I26"/>
       <c s="4" r="J26"/>
       <c s="4" r="K26"/>
       <c s="4" r="L26"/>
@@ -1670,16 +1562,16 @@
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c t="s" s="2" r="B28">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c t="s" s="3" r="C28">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c t="s" s="14" r="D28">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c s="4" r="E28"/>
       <c s="4" r="F28"/>
@@ -1713,11 +1605,9 @@
     </row>
     <row r="29">
       <c t="s" s="5" r="A29">
-        <v>26</v>
+        <v>23</v>
       </c>
-      <c s="5" r="B29">
-        <v>1.0</v>
-      </c>
+      <c s="5" r="B29"/>
       <c s="5" r="C29">
         <v>2.0</v>
       </c>
@@ -1768,9 +1658,7 @@
       <c s="7" r="A30">
         <v>1.0</v>
       </c>
-      <c s="8" r="B30">
-        <v>0.532166</v>
-      </c>
+      <c s="8" r="B30"/>
       <c s="15" r="C30">
         <v>1.514062</v>
       </c>
@@ -1821,9 +1709,7 @@
       <c s="7" r="A31">
         <v>2.0</v>
       </c>
-      <c s="8" r="B31">
-        <v>0.374772</v>
-      </c>
+      <c s="8" r="B31"/>
       <c s="15" r="C31">
         <v>1.512307</v>
       </c>
@@ -1874,9 +1760,7 @@
       <c s="7" r="A32">
         <v>3.0</v>
       </c>
-      <c s="8" r="B32">
-        <v>0.37328</v>
-      </c>
+      <c s="8" r="B32"/>
       <c s="15" r="C32">
         <v>1.515633</v>
       </c>
@@ -1925,38 +1809,35 @@
     </row>
     <row r="33">
       <c t="s" s="9" r="A33">
-        <v>27</v>
+        <v>24</v>
       </c>
-      <c t="str" s="10" r="B33">
-        <f ref="B33:I33" t="shared" si="4">AVERAGE(B30:B32)</f>
-        <v>0.4267393333</v>
-      </c>
+      <c s="10" r="B33"/>
       <c t="str" s="10" r="C33">
-        <f t="shared" si="4"/>
+        <f ref="C33:I33" t="shared" si="5">AVERAGE(C30:C32)</f>
         <v>1.514000667</v>
       </c>
       <c t="str" s="10" r="D33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.612223</v>
       </c>
       <c t="str" s="10" r="E33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.589462</v>
       </c>
       <c t="str" s="10" r="F33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.642394667</v>
       </c>
       <c t="str" s="10" r="G33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.705455667</v>
       </c>
       <c t="str" s="10" r="H33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.770752333</v>
       </c>
       <c t="str" s="10" r="I33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.821922</v>
       </c>
       <c s="6" r="J33"/>
@@ -1986,39 +1867,36 @@
     </row>
     <row r="34">
       <c t="s" s="7" r="A34">
-        <v>28</v>
+        <v>25</v>
       </c>
-      <c t="str" s="11" r="B34">
-        <f>DIVIDE(B33, B33)</f>
+      <c s="11" r="B34"/>
+      <c t="str" s="11" r="C34">
+        <f ref="C34:I34" t="shared" si="6">DIVIDE($C$33, C33)</f>
         <v>1</v>
       </c>
-      <c t="str" s="11" r="C34">
-        <f>DIVIDE(B33, C33)</f>
-        <v>0.2818620511</v>
-      </c>
       <c t="str" s="11" r="D34">
-        <f>DIVIDE(B33, D33)</f>
-        <v>0.264690017</v>
+        <f t="shared" si="6"/>
+        <v>0.9390764594</v>
       </c>
       <c t="str" s="11" r="E34">
-        <f>DIVIDE(B33, E33)</f>
-        <v>0.2684803621</v>
+        <f t="shared" si="6"/>
+        <v>0.9525239777</v>
       </c>
       <c t="str" s="11" r="F34">
-        <f>DIVIDE(B33, F33)</f>
-        <v>0.2598275201</v>
+        <f t="shared" si="6"/>
+        <v>0.9218251236</v>
       </c>
       <c t="str" s="11" r="G34">
-        <f>DIVIDE(B33, G33)</f>
-        <v>0.2502201269</v>
+        <f t="shared" si="6"/>
+        <v>0.8877396793</v>
       </c>
       <c t="str" s="11" r="H34">
-        <f>DIVIDE(B33, H33)</f>
-        <v>0.2409932351</v>
+        <f t="shared" si="6"/>
+        <v>0.8550041913</v>
       </c>
       <c t="str" s="11" r="I34">
-        <f>DIVIDE(B33, I33)</f>
-        <v>0.2342248095</v>
+        <f t="shared" si="6"/>
+        <v>0.8309909352</v>
       </c>
       <c s="6" r="J34"/>
       <c s="6" r="K34"/>
@@ -2046,33 +1924,15 @@
       <c s="6" r="AG34"/>
     </row>
     <row r="35">
-      <c t="s" s="7" r="A35">
-        <v>29</v>
-      </c>
-      <c s="8" r="B35">
-        <v>0.0</v>
-      </c>
-      <c s="12" r="C35">
-        <v>18600.0</v>
-      </c>
-      <c s="12" r="D35">
-        <v>44300.0</v>
-      </c>
-      <c s="12" r="E35">
-        <v>55300.0</v>
-      </c>
-      <c s="12" r="F35">
-        <v>65500.0</v>
-      </c>
-      <c s="12" r="G35">
-        <v>76300.0</v>
-      </c>
-      <c s="12" r="H35">
-        <v>81700.0</v>
-      </c>
-      <c s="12" r="I35">
-        <v>91300.0</v>
-      </c>
+      <c s="7" r="A35"/>
+      <c s="8" r="B35"/>
+      <c s="12" r="C35"/>
+      <c s="12" r="D35"/>
+      <c s="12" r="E35"/>
+      <c s="12" r="F35"/>
+      <c s="12" r="G35"/>
+      <c s="12" r="H35"/>
+      <c s="12" r="I35"/>
       <c s="4" r="J35"/>
       <c s="4" r="K35"/>
       <c s="4" r="L35"/>

</xml_diff>